<commit_message>
Updated Bulk User Add with nric column and reformat some code
</commit_message>
<xml_diff>
--- a/storage/app/public/spreadsheet/Tambah_Pengguna_Baharu.xlsx
+++ b/storage/app/public/spreadsheet/Tambah_Pengguna_Baharu.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">eKV</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t xml:space="preserve">Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Kad Pengenalan</t>
   </si>
   <si>
     <t xml:space="preserve">E-mel</t>
@@ -334,7 +337,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -419,19 +422,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F107"/>
+  <dimension ref="A1:G107"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="A6:F8"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6:G106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="20.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.66"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -444,6 +448,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="23.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
@@ -454,6 +459,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="75.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -466,6 +472,7 @@
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
@@ -486,6 +493,9 @@
       <c r="F5" s="6" t="s">
         <v>9</v>
       </c>
+      <c r="G5" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
@@ -494,6 +504,7 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
@@ -502,6 +513,7 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
@@ -510,6 +522,7 @@
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7"/>
@@ -518,6 +531,7 @@
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
@@ -526,6 +540,7 @@
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7"/>
@@ -534,6 +549,7 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7"/>
@@ -542,6 +558,7 @@
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7"/>
@@ -550,6 +567,7 @@
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7"/>
@@ -558,6 +576,7 @@
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7"/>
@@ -566,6 +585,7 @@
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7"/>
@@ -574,6 +594,7 @@
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7"/>
@@ -582,6 +603,7 @@
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
     </row>
     <row r="18" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7"/>
@@ -590,6 +612,7 @@
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
     </row>
     <row r="19" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7"/>
@@ -598,6 +621,7 @@
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
     </row>
     <row r="20" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7"/>
@@ -606,6 +630,7 @@
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
     </row>
     <row r="21" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7"/>
@@ -614,6 +639,7 @@
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7"/>
@@ -622,6 +648,7 @@
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
     </row>
     <row r="23" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7"/>
@@ -630,6 +657,7 @@
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
     </row>
     <row r="24" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7"/>
@@ -638,6 +666,7 @@
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
     </row>
     <row r="25" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7"/>
@@ -646,6 +675,7 @@
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
     </row>
     <row r="26" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7"/>
@@ -654,6 +684,7 @@
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
     </row>
     <row r="27" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7"/>
@@ -662,6 +693,7 @@
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
     </row>
     <row r="28" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7"/>
@@ -670,6 +702,7 @@
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
     </row>
     <row r="29" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7"/>
@@ -678,6 +711,7 @@
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
     </row>
     <row r="30" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7"/>
@@ -686,6 +720,7 @@
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
     </row>
     <row r="31" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7"/>
@@ -694,6 +729,7 @@
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
     </row>
     <row r="32" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7"/>
@@ -702,6 +738,7 @@
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
     </row>
     <row r="33" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7"/>
@@ -710,6 +747,7 @@
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
     </row>
     <row r="34" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7"/>
@@ -718,6 +756,7 @@
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
     </row>
     <row r="35" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7"/>
@@ -726,6 +765,7 @@
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
     </row>
     <row r="36" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7"/>
@@ -734,6 +774,7 @@
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
     </row>
     <row r="37" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="7"/>
@@ -742,6 +783,7 @@
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
     </row>
     <row r="38" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7"/>
@@ -750,6 +792,7 @@
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
     </row>
     <row r="39" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="7"/>
@@ -758,6 +801,7 @@
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
     </row>
     <row r="40" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="7"/>
@@ -766,6 +810,7 @@
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
     </row>
     <row r="41" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7"/>
@@ -774,6 +819,7 @@
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
     </row>
     <row r="42" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="7"/>
@@ -782,6 +828,7 @@
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
     </row>
     <row r="43" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="7"/>
@@ -790,6 +837,7 @@
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
     </row>
     <row r="44" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="7"/>
@@ -798,6 +846,7 @@
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
     </row>
     <row r="45" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="7"/>
@@ -806,6 +855,7 @@
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
     </row>
     <row r="46" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="7"/>
@@ -814,6 +864,7 @@
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
     </row>
     <row r="47" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="7"/>
@@ -822,6 +873,7 @@
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
     </row>
     <row r="48" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="7"/>
@@ -830,6 +882,7 @@
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
     </row>
     <row r="49" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="7"/>
@@ -838,6 +891,7 @@
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
     </row>
     <row r="50" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="7"/>
@@ -846,6 +900,7 @@
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
     </row>
     <row r="51" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="7"/>
@@ -854,6 +909,7 @@
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
     </row>
     <row r="52" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="7"/>
@@ -862,6 +918,7 @@
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
     </row>
     <row r="53" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="7"/>
@@ -870,6 +927,7 @@
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
     </row>
     <row r="54" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="7"/>
@@ -878,6 +936,7 @@
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
     </row>
     <row r="55" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="7"/>
@@ -886,6 +945,7 @@
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
     </row>
     <row r="56" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="7"/>
@@ -894,6 +954,7 @@
       <c r="D56" s="7"/>
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
     </row>
     <row r="57" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="7"/>
@@ -902,6 +963,7 @@
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
     </row>
     <row r="58" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="7"/>
@@ -910,6 +972,7 @@
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
     </row>
     <row r="59" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="7"/>
@@ -918,6 +981,7 @@
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
     </row>
     <row r="60" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="7"/>
@@ -926,6 +990,7 @@
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
     </row>
     <row r="61" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="7"/>
@@ -934,6 +999,7 @@
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
     </row>
     <row r="62" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="7"/>
@@ -942,6 +1008,7 @@
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
     </row>
     <row r="63" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="7"/>
@@ -950,6 +1017,7 @@
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
     </row>
     <row r="64" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="7"/>
@@ -958,6 +1026,7 @@
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
     </row>
     <row r="65" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="7"/>
@@ -966,6 +1035,7 @@
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
+      <c r="G65" s="7"/>
     </row>
     <row r="66" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="7"/>
@@ -974,6 +1044,7 @@
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
     </row>
     <row r="67" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="7"/>
@@ -982,6 +1053,7 @@
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>
       <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
     </row>
     <row r="68" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="7"/>
@@ -990,6 +1062,7 @@
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
     </row>
     <row r="69" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="7"/>
@@ -998,6 +1071,7 @@
       <c r="D69" s="7"/>
       <c r="E69" s="7"/>
       <c r="F69" s="7"/>
+      <c r="G69" s="7"/>
     </row>
     <row r="70" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="7"/>
@@ -1006,6 +1080,7 @@
       <c r="D70" s="7"/>
       <c r="E70" s="7"/>
       <c r="F70" s="7"/>
+      <c r="G70" s="7"/>
     </row>
     <row r="71" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="7"/>
@@ -1014,6 +1089,7 @@
       <c r="D71" s="7"/>
       <c r="E71" s="7"/>
       <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
     </row>
     <row r="72" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="7"/>
@@ -1022,6 +1098,7 @@
       <c r="D72" s="7"/>
       <c r="E72" s="7"/>
       <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
     </row>
     <row r="73" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="7"/>
@@ -1030,6 +1107,7 @@
       <c r="D73" s="7"/>
       <c r="E73" s="7"/>
       <c r="F73" s="7"/>
+      <c r="G73" s="7"/>
     </row>
     <row r="74" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="7"/>
@@ -1038,6 +1116,7 @@
       <c r="D74" s="7"/>
       <c r="E74" s="7"/>
       <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
     </row>
     <row r="75" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="7"/>
@@ -1046,6 +1125,7 @@
       <c r="D75" s="7"/>
       <c r="E75" s="7"/>
       <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
     </row>
     <row r="76" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="7"/>
@@ -1054,6 +1134,7 @@
       <c r="D76" s="7"/>
       <c r="E76" s="7"/>
       <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
     </row>
     <row r="77" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="7"/>
@@ -1062,6 +1143,7 @@
       <c r="D77" s="7"/>
       <c r="E77" s="7"/>
       <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
     </row>
     <row r="78" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="7"/>
@@ -1070,6 +1152,7 @@
       <c r="D78" s="7"/>
       <c r="E78" s="7"/>
       <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
     </row>
     <row r="79" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="7"/>
@@ -1078,6 +1161,7 @@
       <c r="D79" s="7"/>
       <c r="E79" s="7"/>
       <c r="F79" s="7"/>
+      <c r="G79" s="7"/>
     </row>
     <row r="80" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="7"/>
@@ -1086,6 +1170,7 @@
       <c r="D80" s="7"/>
       <c r="E80" s="7"/>
       <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
     </row>
     <row r="81" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="7"/>
@@ -1094,6 +1179,7 @@
       <c r="D81" s="7"/>
       <c r="E81" s="7"/>
       <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
     </row>
     <row r="82" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="7"/>
@@ -1102,6 +1188,7 @@
       <c r="D82" s="7"/>
       <c r="E82" s="7"/>
       <c r="F82" s="7"/>
+      <c r="G82" s="7"/>
     </row>
     <row r="83" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="7"/>
@@ -1110,6 +1197,7 @@
       <c r="D83" s="7"/>
       <c r="E83" s="7"/>
       <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
     </row>
     <row r="84" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="7"/>
@@ -1118,6 +1206,7 @@
       <c r="D84" s="7"/>
       <c r="E84" s="7"/>
       <c r="F84" s="7"/>
+      <c r="G84" s="7"/>
     </row>
     <row r="85" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="7"/>
@@ -1126,6 +1215,7 @@
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
       <c r="F85" s="7"/>
+      <c r="G85" s="7"/>
     </row>
     <row r="86" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="7"/>
@@ -1134,6 +1224,7 @@
       <c r="D86" s="7"/>
       <c r="E86" s="7"/>
       <c r="F86" s="7"/>
+      <c r="G86" s="7"/>
     </row>
     <row r="87" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="7"/>
@@ -1142,6 +1233,7 @@
       <c r="D87" s="7"/>
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
+      <c r="G87" s="7"/>
     </row>
     <row r="88" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="7"/>
@@ -1150,6 +1242,7 @@
       <c r="D88" s="7"/>
       <c r="E88" s="7"/>
       <c r="F88" s="7"/>
+      <c r="G88" s="7"/>
     </row>
     <row r="89" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="7"/>
@@ -1158,6 +1251,7 @@
       <c r="D89" s="7"/>
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
+      <c r="G89" s="7"/>
     </row>
     <row r="90" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="7"/>
@@ -1166,6 +1260,7 @@
       <c r="D90" s="7"/>
       <c r="E90" s="7"/>
       <c r="F90" s="7"/>
+      <c r="G90" s="7"/>
     </row>
     <row r="91" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="7"/>
@@ -1174,6 +1269,7 @@
       <c r="D91" s="7"/>
       <c r="E91" s="7"/>
       <c r="F91" s="7"/>
+      <c r="G91" s="7"/>
     </row>
     <row r="92" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="7"/>
@@ -1182,6 +1278,7 @@
       <c r="D92" s="7"/>
       <c r="E92" s="7"/>
       <c r="F92" s="7"/>
+      <c r="G92" s="7"/>
     </row>
     <row r="93" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="7"/>
@@ -1190,6 +1287,7 @@
       <c r="D93" s="7"/>
       <c r="E93" s="7"/>
       <c r="F93" s="7"/>
+      <c r="G93" s="7"/>
     </row>
     <row r="94" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="7"/>
@@ -1198,6 +1296,7 @@
       <c r="D94" s="7"/>
       <c r="E94" s="7"/>
       <c r="F94" s="7"/>
+      <c r="G94" s="7"/>
     </row>
     <row r="95" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="7"/>
@@ -1206,6 +1305,7 @@
       <c r="D95" s="7"/>
       <c r="E95" s="7"/>
       <c r="F95" s="7"/>
+      <c r="G95" s="7"/>
     </row>
     <row r="96" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="7"/>
@@ -1214,6 +1314,7 @@
       <c r="D96" s="7"/>
       <c r="E96" s="7"/>
       <c r="F96" s="7"/>
+      <c r="G96" s="7"/>
     </row>
     <row r="97" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="7"/>
@@ -1222,6 +1323,7 @@
       <c r="D97" s="7"/>
       <c r="E97" s="7"/>
       <c r="F97" s="7"/>
+      <c r="G97" s="7"/>
     </row>
     <row r="98" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="7"/>
@@ -1230,6 +1332,7 @@
       <c r="D98" s="7"/>
       <c r="E98" s="7"/>
       <c r="F98" s="7"/>
+      <c r="G98" s="7"/>
     </row>
     <row r="99" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="7"/>
@@ -1238,6 +1341,7 @@
       <c r="D99" s="7"/>
       <c r="E99" s="7"/>
       <c r="F99" s="7"/>
+      <c r="G99" s="7"/>
     </row>
     <row r="100" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="7"/>
@@ -1246,6 +1350,7 @@
       <c r="D100" s="7"/>
       <c r="E100" s="7"/>
       <c r="F100" s="7"/>
+      <c r="G100" s="7"/>
     </row>
     <row r="101" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="7"/>
@@ -1254,6 +1359,7 @@
       <c r="D101" s="7"/>
       <c r="E101" s="7"/>
       <c r="F101" s="7"/>
+      <c r="G101" s="7"/>
     </row>
     <row r="102" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="7"/>
@@ -1262,6 +1368,7 @@
       <c r="D102" s="7"/>
       <c r="E102" s="7"/>
       <c r="F102" s="7"/>
+      <c r="G102" s="7"/>
     </row>
     <row r="103" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="7"/>
@@ -1270,6 +1377,7 @@
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
       <c r="F103" s="7"/>
+      <c r="G103" s="7"/>
     </row>
     <row r="104" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="7"/>
@@ -1278,6 +1386,7 @@
       <c r="D104" s="7"/>
       <c r="E104" s="7"/>
       <c r="F104" s="7"/>
+      <c r="G104" s="7"/>
     </row>
     <row r="105" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="7"/>
@@ -1286,6 +1395,7 @@
       <c r="D105" s="7"/>
       <c r="E105" s="7"/>
       <c r="F105" s="7"/>
+      <c r="G105" s="7"/>
     </row>
     <row r="106" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="7"/>
@@ -1294,6 +1404,7 @@
       <c r="D106" s="7"/>
       <c r="E106" s="7"/>
       <c r="F106" s="7"/>
+      <c r="G106" s="7"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="10"/>
@@ -1304,10 +1415,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C3:G3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>